<commit_message>
This time I know for certain the labels don't overlap!
</commit_message>
<xml_diff>
--- a/Incomes.xlsx
+++ b/Incomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politechnikawroclawska-my.sharepoint.com/personal/282223_student_pwr_edu_pl/Documents/Desktop/Programowanie/AllGitHubRepositories/Income and expense analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{3C6717C2-9BD0-4DCE-B7CD-6358C9AFF513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC43D1AF-845E-4D81-8AF6-027D0CD440B0}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{3C6717C2-9BD0-4DCE-B7CD-6358C9AFF513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E08EE7C-FDBC-443F-BD0E-EBAE4E8904B9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0DB74CF-37C8-4113-AD40-E6C9332CEB9D}"/>
   </bookViews>
@@ -134,6 +134,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -477,7 +481,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
I've computed the expense average for each category and month; computed the frequencies of each category.
</commit_message>
<xml_diff>
--- a/Incomes.xlsx
+++ b/Incomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawel\OneDrive - Politechnika Wroclawska\Desktop\Programowanie\AllGitHubRepositories\Income and expense analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627FF633-B925-462A-AC5C-136B535FD036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF22D41B-7182-48C0-9249-5BA9BB5B5852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0DB74CF-37C8-4113-AD40-E6C9332CEB9D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="11">
   <si>
     <t>Income category</t>
   </si>
@@ -137,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A6B48AB2-A6DD-4987-B1A7-3B44B0E9248C}" name="Table7" displayName="Table7" ref="A1:C92" totalsRowShown="0">
-  <autoFilter ref="A1:C92" xr:uid="{A6B48AB2-A6DD-4987-B1A7-3B44B0E9248C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A6B48AB2-A6DD-4987-B1A7-3B44B0E9248C}" name="Table7" displayName="Table7" ref="A1:C93" totalsRowShown="0">
+  <autoFilter ref="A1:C93" xr:uid="{A6B48AB2-A6DD-4987-B1A7-3B44B0E9248C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B89">
     <sortCondition ref="A1:A89"/>
   </sortState>
@@ -468,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1961AD35-64CA-47EB-87C1-33C307D06AD9}">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1495,6 +1495,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>45711</v>
+      </c>
+      <c r="B93" s="2">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>